<commit_message>
updated meat consumption statistics
</commit_message>
<xml_diff>
--- a/data/data_raw/eurostat/AT_milk_apro_mk_colm.xlsx
+++ b/data/data_raw/eurostat/AT_milk_apro_mk_colm.xlsx
@@ -3684,7 +3684,9 @@
       <c r="PD2" t="n">
         <v>4.02</v>
       </c>
-      <c r="PE2" t="inlineStr"/>
+      <c r="PE2" t="n">
+        <v>4.01</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -4835,7 +4837,9 @@
       <c r="PD3" t="n">
         <v>3.34</v>
       </c>
-      <c r="PE3" t="inlineStr"/>
+      <c r="PE3" t="n">
+        <v>3.36</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -5986,7 +5990,9 @@
       <c r="PD4" t="n">
         <v>275.75</v>
       </c>
-      <c r="PE4" t="inlineStr"/>
+      <c r="PE4" t="n">
+        <v>265.48</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -6727,7 +6733,9 @@
       <c r="PD5" t="n">
         <v>0</v>
       </c>
-      <c r="PE5" t="inlineStr"/>
+      <c r="PE5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -7468,7 +7476,9 @@
       <c r="PD6" t="n">
         <v>0</v>
       </c>
-      <c r="PE6" t="inlineStr"/>
+      <c r="PE6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -8209,7 +8219,9 @@
       <c r="PD7" t="n">
         <v>0</v>
       </c>
-      <c r="PE7" t="inlineStr"/>
+      <c r="PE7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -9360,7 +9372,9 @@
       <c r="PD8" t="n">
         <v>52.87</v>
       </c>
-      <c r="PE8" t="inlineStr"/>
+      <c r="PE8" t="n">
+        <v>51.31</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -10511,7 +10525,9 @@
       <c r="PD9" t="n">
         <v>6.26</v>
       </c>
-      <c r="PE9" t="inlineStr"/>
+      <c r="PE9" t="n">
+        <v>5.82</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -11662,7 +11678,9 @@
       <c r="PD10" t="n">
         <v>0.22</v>
       </c>
-      <c r="PE10" t="inlineStr"/>
+      <c r="PE10" t="n">
+        <v>0.33</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -12813,7 +12831,9 @@
       <c r="PD11" t="n">
         <v>0.44</v>
       </c>
-      <c r="PE11" t="inlineStr"/>
+      <c r="PE11" t="n">
+        <v>0.47</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -14477,7 +14497,9 @@
       <c r="PD13" t="n">
         <v>27.53</v>
       </c>
-      <c r="PE13" t="inlineStr"/>
+      <c r="PE13" t="n">
+        <v>25.87</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -15628,7 +15650,9 @@
       <c r="PD14" t="n">
         <v>2.41</v>
       </c>
-      <c r="PE14" t="inlineStr"/>
+      <c r="PE14" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -16779,7 +16803,9 @@
       <c r="PD15" t="n">
         <v>19.6</v>
       </c>
-      <c r="PE15" t="inlineStr"/>
+      <c r="PE15" t="n">
+        <v>18.12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>